<commit_message>
added err_to_str unit test and fixed calamine engine import
</commit_message>
<xml_diff>
--- a/tests/cell_errors.xlsx
+++ b/tests/cell_errors.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10320"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Felix/DEV/xlwings/xlwings/tests/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fz/Dev/xlwings/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90124BEE-BDE8-8849-81D5-6E37966AF2D1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{008A4D74-EC29-AC4D-8B2F-C0E9BD786ABD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="460" windowWidth="14100" windowHeight="17540" xr2:uid="{4EB32C9D-155D-CA48-B620-FF7DF02BD4A4}"/>
+    <workbookView xWindow="4440" yWindow="-19620" windowWidth="14100" windowHeight="17540" xr2:uid="{4EB32C9D-155D-CA48-B620-FF7DF02BD4A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,6 +26,9 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -412,7 +415,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection sqref="A1:A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>